<commit_message>
export scripts for services,contact,malls, skills. typeahead proto
</commit_message>
<xml_diff>
--- a/data/malls.xlsx
+++ b/data/malls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="Магазины в ТРЦ" sheetId="1" r:id="rId1"/>
+    <sheet name="malls-16" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="343">
   <si>
     <t>Променада</t>
   </si>
@@ -58,9 +58,6 @@
     <t>ARGO CENTER</t>
   </si>
   <si>
-    <t>COLIN’S</t>
-  </si>
-  <si>
     <t>GARCIA JEANS</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t>OGGI</t>
   </si>
   <si>
-    <t>O’STIN</t>
-  </si>
-  <si>
     <t>TIMBERLAND</t>
   </si>
   <si>
@@ -589,9 +583,6 @@
     <t>Tommy Hiffiger</t>
   </si>
   <si>
-    <t>Ostin</t>
-  </si>
-  <si>
     <t>BEST</t>
   </si>
   <si>
@@ -773,9 +764,6 @@
   </si>
   <si>
     <t>Oasis</t>
-  </si>
-  <si>
-    <t>Colin's</t>
   </si>
   <si>
     <t>Topshop</t>
@@ -1066,8 +1054,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1273,8 +1261,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1332,7 +1320,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1367,7 +1355,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1544,21 +1532,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:F59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" style="2" customWidth="1"/>
@@ -1571,1588 +1559,1678 @@
     <col min="9" max="9" width="18.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="42" customHeight="1" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>342</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>346</v>
-      </c>
       <c r="F2" s="9" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>44</v>
+        <v>191</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>197</v>
+        <v>341</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>202</v>
+        <v>124</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>25</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="H6" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>101</v>
+        <v>244</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>345</v>
+        <v>192</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>177</v>
+        <v>239</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>27</v>
+        <v>126</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>206</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="H8" s="10" t="s">
         <v>11</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>243</v>
+        <v>127</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>241</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>244</v>
+        <v>193</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>242</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>245</v>
+        <v>179</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>181</v>
+        <v>243</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C15" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="F13" s="9" t="s">
+      <c r="D16" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G17" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="I13" s="11" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="I19" s="11" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="G21" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>284</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="F16" s="23" t="s">
-        <v>247</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="F17" s="9" t="s">
+      <c r="I21" s="11" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="F22" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="G17" s="9" t="s">
-        <v>286</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="F19" s="9" t="s">
+      <c r="G22" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>287</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>288</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="F22" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="I22" s="11" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="C23" s="2">
         <v>925</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>214</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>215</v>
       </c>
       <c r="F24" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="F27" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="G27" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="G28" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="I24" s="11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>291</v>
-      </c>
-      <c r="I25" s="11" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D26" s="2" t="s">
+      <c r="B29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="I26" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="I27" s="11" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D28" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>219</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="F30" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="E32" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E33" s="6" t="s">
         <v>221</v>
-      </c>
-      <c r="F31" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>222</v>
       </c>
       <c r="F33" s="9" t="s">
         <v>54</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="H33"/>
+      <c r="I33"/>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="H34"/>
+      <c r="I34"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="H35"/>
+      <c r="I35"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2" t="s">
+      <c r="D36" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="H36"/>
+      <c r="I36"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E37" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="F34" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>261</v>
-      </c>
-      <c r="G35" s="13" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="F37" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="H37"/>
+      <c r="I37"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="16" t="s">
+      <c r="D38" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="E38" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="H38"/>
+      <c r="I38"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B39" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="G37" s="9" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2" t="s">
-        <v>155</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>225</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>177</v>
+        <v>245</v>
       </c>
       <c r="G39" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="H39"/>
+      <c r="I39"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="H40"/>
+      <c r="I40"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="H41"/>
+      <c r="I41"/>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="H42"/>
+      <c r="I42"/>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="G43" s="9" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="G40" s="9" t="s">
+      <c r="H43"/>
+      <c r="I43"/>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="B44" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="G44" s="9" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E41" s="6" t="s">
+      <c r="H44"/>
+      <c r="I44"/>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="B45" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="H45"/>
+      <c r="I45"/>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="B46" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="H46"/>
+      <c r="I46"/>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="B47" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E47" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="F41" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B43" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="F43" s="9" t="s">
+      <c r="F47" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="G43" s="9" t="s">
+      <c r="G47" s="9" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E44" s="6" t="s">
+      <c r="H47"/>
+      <c r="I47"/>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="B48" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E48" s="6" t="s">
         <v>204</v>
-      </c>
-      <c r="F44" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="G44" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="G45" s="9" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="F46" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="G46" s="9" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="F47" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="G47" s="9" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>230</v>
       </c>
       <c r="F48" s="9" t="s">
         <v>72</v>
       </c>
       <c r="G48" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="H48"/>
+      <c r="I48"/>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49"/>
+      <c r="B49" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E49" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="H49"/>
+      <c r="I49"/>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50"/>
+      <c r="B50" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="H50"/>
+      <c r="I50"/>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51"/>
+      <c r="B51" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G51" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="H51"/>
+      <c r="I51"/>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52"/>
+      <c r="B52" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="G52" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="H52"/>
+      <c r="I52"/>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53"/>
+      <c r="B53" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="F53" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="G53" s="9" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="49" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="F49" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="G49" s="9" t="s">
+      <c r="H53"/>
+      <c r="I53"/>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54"/>
+      <c r="B54" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="G54" s="9" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="50" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="F50" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="G50" s="9" t="s">
+      <c r="H54"/>
+      <c r="I54"/>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55"/>
+      <c r="B55" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="G55" s="9" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="51" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="F51" s="9" t="s">
-        <v>267</v>
-      </c>
-      <c r="G51" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="52" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C52" s="2"/>
-      <c r="D52" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="F52" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="G52" s="9" t="s">
+      <c r="H55"/>
+      <c r="I55"/>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56"/>
+      <c r="D56" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G56" s="9" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="53" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="F53" s="9" t="s">
+      <c r="H56"/>
+      <c r="I56"/>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57"/>
+      <c r="D57" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E57" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F57" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="G53" s="9" t="s">
+      <c r="G57" s="9" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="54" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E54" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="F54" s="30" t="s">
-        <v>269</v>
-      </c>
-      <c r="G54" s="9" t="s">
+      <c r="H57"/>
+      <c r="I57"/>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58"/>
+      <c r="D58" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F58" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G58" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H58"/>
+      <c r="I58"/>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59"/>
+      <c r="D59" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="G59" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H59"/>
+      <c r="I59"/>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60"/>
+      <c r="D60" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G60" s="9" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="55" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F55" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="G55" s="9" t="s">
+      <c r="H60"/>
+      <c r="I60"/>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61"/>
+      <c r="D61" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="G61" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="H61"/>
+      <c r="I61"/>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62"/>
+      <c r="D62" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G62" s="9" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="56" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="F56" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="G56" s="9" t="s">
+      <c r="H62"/>
+      <c r="I62"/>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63"/>
+      <c r="D63" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G63" s="9" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="57" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="F57" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="G57" s="9" t="s">
+      <c r="H63"/>
+      <c r="I63"/>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64"/>
+      <c r="D64" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G64" s="9" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="58" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="F58" s="9" t="s">
-        <v>272</v>
-      </c>
-      <c r="G58" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="F59" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="G59" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="60" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="F60" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="G60" s="9" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="61" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="F61" s="9"/>
-      <c r="G61" s="9" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="62" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E62" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="F62" s="9"/>
-      <c r="G62" s="9" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="63" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E63" s="9"/>
-      <c r="F63" s="9"/>
-      <c r="G63" s="9" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="64" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E64" s="9"/>
-      <c r="F64" s="9"/>
-      <c r="G64" s="9" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="65" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H64"/>
+      <c r="I64"/>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65"/>
+      <c r="B65"/>
+      <c r="C65"/>
       <c r="D65" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E65" s="9"/>
-      <c r="F65" s="9"/>
       <c r="G65" s="9" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="66" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+      <c r="H65"/>
+      <c r="I65"/>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66"/>
+      <c r="B66"/>
+      <c r="C66"/>
       <c r="D66" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E66" s="9"/>
-      <c r="F66" s="9"/>
+        <v>93</v>
+      </c>
       <c r="G66" s="28" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="67" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="H66"/>
+      <c r="I66"/>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67"/>
+      <c r="B67"/>
+      <c r="C67"/>
       <c r="D67" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="G67" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="H67"/>
+      <c r="I67"/>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68"/>
+      <c r="B68"/>
+      <c r="C68"/>
+      <c r="D68" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="H68"/>
+      <c r="I68"/>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69"/>
+      <c r="B69"/>
+      <c r="C69"/>
+      <c r="D69" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E67" s="9"/>
-      <c r="F67" s="9"/>
-      <c r="G67" s="9" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="68" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D68" s="2" t="s">
+      <c r="H69"/>
+      <c r="I69"/>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70"/>
+      <c r="B70"/>
+      <c r="C70"/>
+      <c r="D70" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E68" s="9"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
-    </row>
-    <row r="69" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D69" s="2" t="s">
+      <c r="H70"/>
+      <c r="I70"/>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71"/>
+      <c r="B71"/>
+      <c r="C71"/>
+      <c r="D71" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="E69" s="9"/>
-      <c r="F69" s="9"/>
-      <c r="G69" s="9"/>
-    </row>
-    <row r="70" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D70" s="2" t="s">
+      <c r="H71"/>
+      <c r="I71"/>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72"/>
+      <c r="B72"/>
+      <c r="C72"/>
+      <c r="D72" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="E70" s="9"/>
-      <c r="F70" s="9"/>
-      <c r="G70" s="9"/>
-    </row>
-    <row r="71" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D71" s="2" t="s">
+      <c r="H72"/>
+      <c r="I72"/>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73"/>
+      <c r="B73"/>
+      <c r="C73"/>
+      <c r="D73" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E71" s="9"/>
-      <c r="F71" s="9"/>
-      <c r="G71" s="9"/>
-    </row>
-    <row r="72" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D72" s="2" t="s">
+      <c r="H73"/>
+      <c r="I73"/>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74"/>
+      <c r="B74"/>
+      <c r="C74"/>
+      <c r="D74" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="E72" s="9"/>
-      <c r="F72" s="9"/>
-      <c r="G72" s="9"/>
-    </row>
-    <row r="73" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D73" s="2" t="s">
+      <c r="H74"/>
+      <c r="I74"/>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75"/>
+      <c r="B75"/>
+      <c r="C75"/>
+      <c r="D75" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="E73" s="9"/>
-      <c r="F73" s="9"/>
-      <c r="G73" s="9"/>
-    </row>
-    <row r="74" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D74" s="2" t="s">
+      <c r="H75"/>
+      <c r="I75"/>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76"/>
+      <c r="B76"/>
+      <c r="C76"/>
+      <c r="D76" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H76"/>
+      <c r="I76"/>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77"/>
+      <c r="B77"/>
+      <c r="C77"/>
+      <c r="D77" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E74" s="9"/>
-      <c r="F74" s="9"/>
-      <c r="G74" s="9"/>
-    </row>
-    <row r="75" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D75" s="2" t="s">
+      <c r="H77"/>
+      <c r="I77"/>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78"/>
+      <c r="B78"/>
+      <c r="C78"/>
+      <c r="D78" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E75" s="9"/>
-      <c r="F75" s="9"/>
-      <c r="G75" s="9"/>
-    </row>
-    <row r="76" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D76" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E76" s="9"/>
-      <c r="F76" s="9"/>
-      <c r="G76" s="9"/>
-    </row>
-    <row r="77" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D77" s="2" t="s">
+      <c r="H78"/>
+      <c r="I78"/>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79"/>
+      <c r="B79"/>
+      <c r="C79"/>
+      <c r="D79" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="E77" s="9"/>
-      <c r="F77" s="9"/>
-      <c r="G77" s="9"/>
-    </row>
-    <row r="78" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D78" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E78" s="9"/>
-      <c r="F78" s="9"/>
-      <c r="G78" s="9"/>
-    </row>
-    <row r="79" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D79" s="2" t="s">
+      <c r="H79"/>
+      <c r="I79"/>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80"/>
+      <c r="B80"/>
+      <c r="C80"/>
+      <c r="D80" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="E79" s="9"/>
-      <c r="F79" s="9"/>
-      <c r="G79" s="9"/>
-    </row>
-    <row r="80" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D80" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E80" s="9"/>
-      <c r="F80" s="9"/>
-      <c r="G80" s="9"/>
-    </row>
-    <row r="81" spans="4:4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H80"/>
+      <c r="I80"/>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81"/>
+      <c r="B81"/>
+      <c r="C81"/>
       <c r="D81" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="82" spans="4:4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="E81"/>
+      <c r="F81"/>
+      <c r="G81"/>
+      <c r="H81"/>
+      <c r="I81"/>
+    </row>
+    <row r="82" spans="1:9">
+      <c r="A82"/>
+      <c r="B82"/>
+      <c r="C82"/>
       <c r="D82" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="83" spans="4:4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D83" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="84" spans="4:4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D84" s="18" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="85" spans="4:4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="E82"/>
+      <c r="F82"/>
+      <c r="G82"/>
+      <c r="H82"/>
+      <c r="I82"/>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="A83"/>
+      <c r="B83"/>
+      <c r="C83"/>
+      <c r="D83" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="E83"/>
+      <c r="F83"/>
+      <c r="G83"/>
+      <c r="H83"/>
+      <c r="I83"/>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84"/>
+      <c r="B84"/>
+      <c r="C84"/>
+      <c r="D84" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E84"/>
+      <c r="F84"/>
+      <c r="G84"/>
+      <c r="H84"/>
+      <c r="I84"/>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85"/>
+      <c r="B85"/>
+      <c r="C85"/>
       <c r="D85" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="86" spans="4:4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D86" s="2" t="s">
-        <v>74</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="E85"/>
+      <c r="F85"/>
+      <c r="G85"/>
+      <c r="H85"/>
+      <c r="I85"/>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86"/>
+      <c r="B86"/>
+      <c r="C86"/>
+      <c r="E86"/>
+      <c r="F86"/>
+      <c r="G86"/>
+      <c r="H86"/>
+      <c r="I86"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3160,68 +3238,67 @@
     <hyperlink ref="A40" r:id="rId2" display="http://www.promenada.com.ua/uk/all-promenada/shops/mariella-rosatti.html"/>
     <hyperlink ref="B5" r:id="rId3" display="http://dreamtown.ua/shop/extyn_junker"/>
     <hyperlink ref="B20" r:id="rId4" display="http://dreamtown.ua/shop/sisley"/>
-    <hyperlink ref="E18" r:id="rId5" display="javascript:void(0);"/>
-    <hyperlink ref="E19" r:id="rId6" display="javascript:void(0);"/>
-    <hyperlink ref="E20" r:id="rId7" display="javascript:void(0);"/>
-    <hyperlink ref="E21" r:id="rId8" display="javascript:void(0);"/>
-    <hyperlink ref="E22" r:id="rId9" display="javascript:void(0);"/>
-    <hyperlink ref="E23" r:id="rId10" display="javascript:void(0);"/>
-    <hyperlink ref="E24" r:id="rId11" display="javascript:void(0);"/>
-    <hyperlink ref="E25" r:id="rId12" display="javascript:void(0);"/>
-    <hyperlink ref="E26" r:id="rId13" display="javascript:void(0);"/>
-    <hyperlink ref="E27" r:id="rId14" display="javascript:void(0);"/>
-    <hyperlink ref="E28" r:id="rId15" display="javascript:void(0);"/>
-    <hyperlink ref="E29" r:id="rId16" display="javascript:void(0);"/>
-    <hyperlink ref="E30" r:id="rId17" display="javascript:void(0);"/>
-    <hyperlink ref="E31" r:id="rId18" display="javascript:void(0);"/>
-    <hyperlink ref="E32" r:id="rId19" display="javascript:void(0);"/>
-    <hyperlink ref="E33" r:id="rId20" display="javascript:void(0);"/>
-    <hyperlink ref="E34" r:id="rId21" display="javascript:void(0);"/>
-    <hyperlink ref="E35" r:id="rId22" display="javascript:void(0);"/>
-    <hyperlink ref="E36" r:id="rId23" display="javascript:void(0);"/>
-    <hyperlink ref="E37" r:id="rId24" display="javascript:void(0);"/>
-    <hyperlink ref="E38" r:id="rId25" display="javascript:void(0);"/>
-    <hyperlink ref="E39" r:id="rId26" display="javascript:void(0);"/>
-    <hyperlink ref="E40" r:id="rId27" display="javascript:void(0);"/>
-    <hyperlink ref="E41" r:id="rId28" display="javascript:void(0);"/>
-    <hyperlink ref="E42" r:id="rId29" display="javascript:void(0);"/>
-    <hyperlink ref="E43" r:id="rId30" display="javascript:void(0);"/>
-    <hyperlink ref="E44" r:id="rId31" display="javascript:void(0);"/>
-    <hyperlink ref="E45" r:id="rId32" display="javascript:void(0);"/>
-    <hyperlink ref="E46" r:id="rId33" display="javascript:void(0);"/>
-    <hyperlink ref="E47" r:id="rId34" display="javascript:void(0);"/>
-    <hyperlink ref="E48" r:id="rId35" display="javascript:void(0);"/>
-    <hyperlink ref="E49" r:id="rId36" display="javascript:void(0);"/>
-    <hyperlink ref="E50" r:id="rId37" display="javascript:void(0);"/>
-    <hyperlink ref="E51" r:id="rId38" display="javascript:void(0);"/>
-    <hyperlink ref="E52" r:id="rId39" display="javascript:void(0);"/>
-    <hyperlink ref="E53" r:id="rId40" display="javascript:void(0);"/>
-    <hyperlink ref="E54" r:id="rId41" display="javascript:void(0);"/>
-    <hyperlink ref="E55" r:id="rId42" display="javascript:void(0);"/>
-    <hyperlink ref="E56" r:id="rId43" display="javascript:void(0);"/>
-    <hyperlink ref="E57" r:id="rId44" display="javascript:void(0);"/>
-    <hyperlink ref="E58" r:id="rId45" display="javascript:void(0);"/>
-    <hyperlink ref="E59" r:id="rId46" display="javascript:void(0);"/>
-    <hyperlink ref="E60" r:id="rId47" display="javascript:void(0);"/>
-    <hyperlink ref="E61" r:id="rId48" display="javascript:void(0);"/>
-    <hyperlink ref="E62" r:id="rId49" display="javascript:void(0);"/>
-    <hyperlink ref="F16" r:id="rId50" display="http://skymall.ua/79-ostin.html"/>
-    <hyperlink ref="F54" r:id="rId51" display="http://skymall.ua/8-adidas.html"/>
+    <hyperlink ref="E14" r:id="rId5" display="javascript:void(0);"/>
+    <hyperlink ref="E15" r:id="rId6" display="javascript:void(0);"/>
+    <hyperlink ref="E16" r:id="rId7" display="javascript:void(0);"/>
+    <hyperlink ref="E17" r:id="rId8" display="javascript:void(0);"/>
+    <hyperlink ref="E18" r:id="rId9" display="javascript:void(0);"/>
+    <hyperlink ref="E19" r:id="rId10" display="javascript:void(0);"/>
+    <hyperlink ref="E20" r:id="rId11" display="javascript:void(0);"/>
+    <hyperlink ref="E21" r:id="rId12" display="javascript:void(0);"/>
+    <hyperlink ref="E22" r:id="rId13" display="javascript:void(0);"/>
+    <hyperlink ref="E23" r:id="rId14" display="javascript:void(0);"/>
+    <hyperlink ref="E24" r:id="rId15" display="javascript:void(0);"/>
+    <hyperlink ref="E25" r:id="rId16" display="javascript:void(0);"/>
+    <hyperlink ref="E26" r:id="rId17" display="javascript:void(0);"/>
+    <hyperlink ref="E27" r:id="rId18" display="javascript:void(0);"/>
+    <hyperlink ref="E28" r:id="rId19" display="javascript:void(0);"/>
+    <hyperlink ref="E29" r:id="rId20" display="javascript:void(0);"/>
+    <hyperlink ref="E30" r:id="rId21" display="javascript:void(0);"/>
+    <hyperlink ref="E31" r:id="rId22" display="javascript:void(0);"/>
+    <hyperlink ref="E32" r:id="rId23" display="javascript:void(0);"/>
+    <hyperlink ref="E33" r:id="rId24" display="javascript:void(0);"/>
+    <hyperlink ref="E34" r:id="rId25" display="javascript:void(0);"/>
+    <hyperlink ref="E35" r:id="rId26" display="javascript:void(0);"/>
+    <hyperlink ref="E36" r:id="rId27" display="javascript:void(0);"/>
+    <hyperlink ref="E37" r:id="rId28" display="javascript:void(0);"/>
+    <hyperlink ref="E38" r:id="rId29" display="javascript:void(0);"/>
+    <hyperlink ref="E39" r:id="rId30" display="javascript:void(0);"/>
+    <hyperlink ref="E40" r:id="rId31" display="javascript:void(0);"/>
+    <hyperlink ref="E41" r:id="rId32" display="javascript:void(0);"/>
+    <hyperlink ref="E42" r:id="rId33" display="javascript:void(0);"/>
+    <hyperlink ref="E43" r:id="rId34" display="javascript:void(0);"/>
+    <hyperlink ref="E44" r:id="rId35" display="javascript:void(0);"/>
+    <hyperlink ref="E45" r:id="rId36" display="javascript:void(0);"/>
+    <hyperlink ref="E46" r:id="rId37" display="javascript:void(0);"/>
+    <hyperlink ref="E47" r:id="rId38" display="javascript:void(0);"/>
+    <hyperlink ref="E48" r:id="rId39" display="javascript:void(0);"/>
+    <hyperlink ref="E49" r:id="rId40" display="javascript:void(0);"/>
+    <hyperlink ref="E50" r:id="rId41" display="javascript:void(0);"/>
+    <hyperlink ref="E51" r:id="rId42" display="javascript:void(0);"/>
+    <hyperlink ref="E52" r:id="rId43" display="javascript:void(0);"/>
+    <hyperlink ref="E53" r:id="rId44" display="javascript:void(0);"/>
+    <hyperlink ref="E54" r:id="rId45" display="javascript:void(0);"/>
+    <hyperlink ref="E55" r:id="rId46" display="javascript:void(0);"/>
+    <hyperlink ref="E56" r:id="rId47" display="javascript:void(0);"/>
+    <hyperlink ref="E57" r:id="rId48" display="javascript:void(0);"/>
+    <hyperlink ref="F15" r:id="rId49" display="http://skymall.ua/79-ostin.html"/>
+    <hyperlink ref="F53" r:id="rId50" display="http://skymall.ua/8-adidas.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId52"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId51"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I5" sqref="I5:I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" style="2" customWidth="1"/>
@@ -3234,292 +3311,292 @@
     <col min="9" max="9" width="18.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="42" customHeight="1" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>342</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>346</v>
-      </c>
       <c r="F2" s="9" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="B5" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="I5" s="10"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="B6" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H6" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I6" s="11"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="3"/>
       <c r="C7" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I7" s="11"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="C8" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="9" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H8" s="10" t="s">
         <v>11</v>
       </c>
       <c r="I8" s="11"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="C9" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I9" s="11"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="12"/>
       <c r="F10" s="19"/>
       <c r="I10" s="11"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="I11" s="11"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" s="12"/>
       <c r="I12" s="11"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="E13" s="17"/>
       <c r="I13" s="11"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="16"/>
       <c r="C14" s="12"/>
       <c r="I14" s="11"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="I15" s="11"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="F16" s="23"/>
       <c r="I16" s="11"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="I17" s="11"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="16"/>
       <c r="B18" s="26"/>
       <c r="E18" s="6"/>
       <c r="I18" s="11"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="E19" s="6"/>
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="B20" s="3"/>
       <c r="C20" s="24"/>
       <c r="E20" s="6"/>
       <c r="I20" s="11"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="E21" s="6"/>
       <c r="I21" s="11"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="15"/>
       <c r="C22" s="27"/>
       <c r="E22" s="6"/>
       <c r="F22" s="17"/>
       <c r="I22" s="11"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="18"/>
       <c r="E23" s="6"/>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="E24" s="6"/>
       <c r="I24" s="11"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="E25" s="6"/>
       <c r="I25" s="11"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="E26" s="6"/>
       <c r="I26" s="11"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27" s="20"/>
       <c r="E27" s="6"/>
       <c r="I27" s="11"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="D28" s="27"/>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="E29" s="6"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30" s="24"/>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="E31" s="6"/>
       <c r="F31" s="22"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" customFormat="1">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -3528,7 +3605,7 @@
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
     </row>
-    <row r="34" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" customFormat="1">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -3537,7 +3614,7 @@
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
     </row>
-    <row r="35" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" customFormat="1">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -3546,7 +3623,7 @@
       <c r="F35" s="9"/>
       <c r="G35" s="13"/>
     </row>
-    <row r="36" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" customFormat="1">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -3555,7 +3632,7 @@
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
     </row>
-    <row r="37" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" customFormat="1">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -3564,7 +3641,7 @@
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
     </row>
-    <row r="38" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" customFormat="1">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -3573,7 +3650,7 @@
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
     </row>
-    <row r="39" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" customFormat="1">
       <c r="A39" s="2"/>
       <c r="B39" s="12"/>
       <c r="C39" s="2"/>
@@ -3582,7 +3659,7 @@
       <c r="F39" s="9"/>
       <c r="G39" s="9"/>
     </row>
-    <row r="40" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" customFormat="1">
       <c r="A40" s="3"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -3591,7 +3668,7 @@
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
     </row>
-    <row r="41" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" customFormat="1">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -3600,7 +3677,7 @@
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
     </row>
-    <row r="42" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" customFormat="1">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -3609,7 +3686,7 @@
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
     </row>
-    <row r="43" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" customFormat="1">
       <c r="A43" s="2"/>
       <c r="B43" s="24"/>
       <c r="C43" s="2"/>
@@ -3618,7 +3695,7 @@
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
     </row>
-    <row r="44" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" customFormat="1">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -3627,7 +3704,7 @@
       <c r="F44" s="13"/>
       <c r="G44" s="9"/>
     </row>
-    <row r="45" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" customFormat="1">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -3636,7 +3713,7 @@
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
     </row>
-    <row r="46" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" customFormat="1">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -3645,7 +3722,7 @@
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
     </row>
-    <row r="47" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" customFormat="1">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -3654,7 +3731,7 @@
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
     </row>
-    <row r="48" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" customFormat="1">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -3663,7 +3740,7 @@
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
     </row>
-    <row r="49" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7" customFormat="1">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -3671,7 +3748,7 @@
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
     </row>
-    <row r="50" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" customFormat="1">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -3679,7 +3756,7 @@
       <c r="F50" s="9"/>
       <c r="G50" s="9"/>
     </row>
-    <row r="51" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7" customFormat="1">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -3687,7 +3764,7 @@
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
     </row>
-    <row r="52" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:7" customFormat="1">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="12"/>
@@ -3695,7 +3772,7 @@
       <c r="F52" s="9"/>
       <c r="G52" s="9"/>
     </row>
-    <row r="53" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:7" customFormat="1">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -3703,7 +3780,7 @@
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
     </row>
-    <row r="54" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7" customFormat="1">
       <c r="B54" s="27"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -3711,7 +3788,7 @@
       <c r="F54" s="30"/>
       <c r="G54" s="9"/>
     </row>
-    <row r="55" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7" customFormat="1">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -3719,7 +3796,7 @@
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
     </row>
-    <row r="56" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7" customFormat="1">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -3727,7 +3804,7 @@
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
     </row>
-    <row r="57" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:7" customFormat="1">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -3735,7 +3812,7 @@
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
     </row>
-    <row r="58" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:7" customFormat="1">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -3743,7 +3820,7 @@
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
     </row>
-    <row r="59" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:7" customFormat="1">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -3751,7 +3828,7 @@
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
     </row>
-    <row r="60" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:7" customFormat="1">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -3759,7 +3836,7 @@
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
     </row>
-    <row r="61" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:7" customFormat="1">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -3767,7 +3844,7 @@
       <c r="F61" s="9"/>
       <c r="G61" s="9"/>
     </row>
-    <row r="62" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:7" customFormat="1">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -3775,7 +3852,7 @@
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
     </row>
-    <row r="63" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:7" customFormat="1">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -3783,7 +3860,7 @@
       <c r="F63" s="9"/>
       <c r="G63" s="9"/>
     </row>
-    <row r="64" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:7" customFormat="1">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -3791,118 +3868,118 @@
       <c r="F64" s="9"/>
       <c r="G64" s="9"/>
     </row>
-    <row r="65" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:7" customFormat="1">
       <c r="D65" s="2"/>
       <c r="E65" s="9"/>
       <c r="F65" s="9"/>
       <c r="G65" s="9"/>
     </row>
-    <row r="66" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:7" customFormat="1">
       <c r="D66" s="2"/>
       <c r="E66" s="9"/>
       <c r="F66" s="9"/>
       <c r="G66" s="28"/>
     </row>
-    <row r="67" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:7" customFormat="1">
       <c r="D67" s="2"/>
       <c r="E67" s="9"/>
       <c r="F67" s="9"/>
       <c r="G67" s="9"/>
     </row>
-    <row r="68" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:7" customFormat="1">
       <c r="D68" s="2"/>
       <c r="E68" s="9"/>
       <c r="F68" s="9"/>
       <c r="G68" s="9"/>
     </row>
-    <row r="69" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:7" customFormat="1">
       <c r="D69" s="2"/>
       <c r="E69" s="9"/>
       <c r="F69" s="9"/>
       <c r="G69" s="9"/>
     </row>
-    <row r="70" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:7" customFormat="1">
       <c r="D70" s="2"/>
       <c r="E70" s="9"/>
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
     </row>
-    <row r="71" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:7" customFormat="1">
       <c r="D71" s="2"/>
       <c r="E71" s="9"/>
       <c r="F71" s="9"/>
       <c r="G71" s="9"/>
     </row>
-    <row r="72" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:7" customFormat="1">
       <c r="D72" s="2"/>
       <c r="E72" s="9"/>
       <c r="F72" s="9"/>
       <c r="G72" s="9"/>
     </row>
-    <row r="73" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:7" customFormat="1">
       <c r="D73" s="2"/>
       <c r="E73" s="9"/>
       <c r="F73" s="9"/>
       <c r="G73" s="9"/>
     </row>
-    <row r="74" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:7" customFormat="1">
       <c r="D74" s="2"/>
       <c r="E74" s="9"/>
       <c r="F74" s="9"/>
       <c r="G74" s="9"/>
     </row>
-    <row r="75" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:7" customFormat="1">
       <c r="D75" s="2"/>
       <c r="E75" s="9"/>
       <c r="F75" s="9"/>
       <c r="G75" s="9"/>
     </row>
-    <row r="76" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:7" customFormat="1">
       <c r="D76" s="2"/>
       <c r="E76" s="9"/>
       <c r="F76" s="9"/>
       <c r="G76" s="9"/>
     </row>
-    <row r="77" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:7" customFormat="1">
       <c r="D77" s="2"/>
       <c r="E77" s="9"/>
       <c r="F77" s="9"/>
       <c r="G77" s="9"/>
     </row>
-    <row r="78" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:7" customFormat="1">
       <c r="D78" s="2"/>
       <c r="E78" s="9"/>
       <c r="F78" s="9"/>
       <c r="G78" s="9"/>
     </row>
-    <row r="79" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:7" customFormat="1">
       <c r="D79" s="2"/>
       <c r="E79" s="9"/>
       <c r="F79" s="9"/>
       <c r="G79" s="9"/>
     </row>
-    <row r="80" spans="4:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:7" customFormat="1">
       <c r="D80" s="2"/>
       <c r="E80" s="9"/>
       <c r="F80" s="9"/>
       <c r="G80" s="9"/>
     </row>
-    <row r="81" spans="4:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:4" customFormat="1">
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="4:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:4" customFormat="1">
       <c r="D82" s="2"/>
     </row>
-    <row r="83" spans="4:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:4" customFormat="1">
       <c r="D83" s="2"/>
     </row>
-    <row r="84" spans="4:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:4" customFormat="1">
       <c r="D84" s="18"/>
     </row>
-    <row r="85" spans="4:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:4" customFormat="1">
       <c r="D85" s="2"/>
     </row>
-    <row r="86" spans="4:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:4" customFormat="1">
       <c r="D86" s="2"/>
     </row>
   </sheetData>

</xml_diff>